<commit_message>
Updated by Kamna on 24 Aug
</commit_message>
<xml_diff>
--- a/Knowledge Enhancement Plan for the team- draft.xlsx
+++ b/Knowledge Enhancement Plan for the team- draft.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="17329"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20730"/>
+  <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\AB77588\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\GITHUB\KamnaGupta\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{33E0DD4A-571B-4019-BFA0-96A8770D52EE}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="6930"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="6930" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -24,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="44">
   <si>
     <t>Srinivas</t>
   </si>
@@ -209,11 +210,23 @@
   <si>
     <t>Latest status as on 5/23</t>
   </si>
+  <si>
+    <t>Latest status as on 5/24</t>
+  </si>
+  <si>
+    <t>GiTHub document is added and sent for Review. Working DatabaseTesting related document with Ramesh</t>
+  </si>
+  <si>
+    <t>On Leave</t>
+  </si>
+  <si>
+    <t>Introduction to RPA,  Introduction to UI Path and Installed UI path tool</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -289,7 +302,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -319,6 +332,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -633,11 +649,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H7"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:I7"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
-      <selection activeCell="H1" sqref="H1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K6" sqref="K6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -648,10 +664,10 @@
     <col min="5" max="5" width="59" style="1" customWidth="1"/>
     <col min="6" max="6" width="33" style="1" customWidth="1"/>
     <col min="7" max="7" width="38.5703125" customWidth="1"/>
-    <col min="8" max="8" width="20.42578125" customWidth="1"/>
+    <col min="8" max="9" width="20.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>4</v>
       </c>
@@ -676,8 +692,11 @@
       <c r="H1" s="9" t="s">
         <v>39</v>
       </c>
+      <c r="I1" s="9" t="s">
+        <v>40</v>
+      </c>
     </row>
-    <row r="2" spans="1:8" ht="270" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9" ht="90" x14ac:dyDescent="0.25">
       <c r="A2" s="4">
         <v>1</v>
       </c>
@@ -702,8 +721,11 @@
       <c r="H2" s="10" t="s">
         <v>37</v>
       </c>
+      <c r="I2" s="10" t="s">
+        <v>37</v>
+      </c>
     </row>
-    <row r="3" spans="1:8" ht="270" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:9" ht="90" x14ac:dyDescent="0.25">
       <c r="A3" s="4">
         <v>2</v>
       </c>
@@ -728,8 +750,11 @@
       <c r="H3" s="10" t="s">
         <v>38</v>
       </c>
+      <c r="I3" s="10" t="s">
+        <v>38</v>
+      </c>
     </row>
-    <row r="4" spans="1:8" ht="135" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:9" ht="135" x14ac:dyDescent="0.25">
       <c r="A4" s="4">
         <v>3</v>
       </c>
@@ -752,7 +777,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="5" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:9" ht="60" x14ac:dyDescent="0.25">
       <c r="A5" s="4">
         <v>4</v>
       </c>
@@ -774,8 +799,11 @@
       <c r="G5" s="11" t="s">
         <v>36</v>
       </c>
+      <c r="I5" s="10" t="s">
+        <v>43</v>
+      </c>
     </row>
-    <row r="6" spans="1:8" ht="75" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:9" ht="90" x14ac:dyDescent="0.25">
       <c r="A6" s="4">
         <v>5</v>
       </c>
@@ -797,8 +825,14 @@
       <c r="G6" s="1" t="s">
         <v>35</v>
       </c>
+      <c r="H6" s="12" t="s">
+        <v>42</v>
+      </c>
+      <c r="I6" s="12" t="s">
+        <v>41</v>
+      </c>
     </row>
-    <row r="7" spans="1:8" ht="60" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:9" ht="60" x14ac:dyDescent="0.25">
       <c r="A7" s="4">
         <v>6</v>
       </c>

</xml_diff>

<commit_message>
updated for Kamna and Ramesh on 28th May
</commit_message>
<xml_diff>
--- a/Knowledge Enhancement Plan for the team- draft.xlsx
+++ b/Knowledge Enhancement Plan for the team- draft.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\GITHUB\KamnaGupta\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B051E334-3693-4A13-B54D-F2B610D263DB}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{23B27D73-A1CA-4612-ABD2-17FA4B5C3976}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="6930" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="54">
   <si>
     <t>Srinivas</t>
   </si>
@@ -228,9 +228,6 @@
 3. Writing of step definitions is in progress.</t>
   </si>
   <si>
-    <t>Latest status as on 5/25</t>
-  </si>
-  <si>
     <t>1.       STAF framework is in progress
 2.       Adhoc Request that are worked  for Today :
 1.       Consolidated “Testing Achievements - 2018-19” for STR
@@ -252,6 +249,18 @@
     <t>Working on Database testing document.
 Studying shell Scripting.
 I have scheduled a unix session .</t>
+  </si>
+  <si>
+    <t>Learning shell scripting/PPT preparation/Demo</t>
+  </si>
+  <si>
+    <t>Latest status as on 5/27</t>
+  </si>
+  <si>
+    <t>Latest status as on 5/28</t>
+  </si>
+  <si>
+    <t>Learned Python Arithmetic and Assignment operators &amp; practiced the same by writing small programs.</t>
   </si>
 </sst>
 </file>
@@ -295,7 +304,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="3">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -329,6 +338,19 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -358,14 +380,14 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -681,10 +703,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:J7"/>
+  <dimension ref="A1:K7"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E5" workbookViewId="0">
-      <selection activeCell="J8" sqref="J8"/>
+    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
+      <selection activeCell="K5" sqref="K5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -698,9 +720,10 @@
     <col min="8" max="8" width="20.42578125" customWidth="1"/>
     <col min="9" max="9" width="32.42578125" customWidth="1"/>
     <col min="10" max="10" width="25" customWidth="1"/>
+    <col min="11" max="11" width="24.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" ht="30" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>4</v>
       </c>
@@ -716,7 +739,7 @@
       <c r="E1" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="F1" s="3" t="s">
+      <c r="F1" s="10" t="s">
         <v>9</v>
       </c>
       <c r="G1" s="9" t="s">
@@ -729,10 +752,13 @@
         <v>40</v>
       </c>
       <c r="J1" s="9" t="s">
-        <v>45</v>
+        <v>51</v>
+      </c>
+      <c r="K1" s="9" t="s">
+        <v>52</v>
       </c>
     </row>
-    <row r="2" spans="1:10" ht="180" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:11" ht="180" x14ac:dyDescent="0.25">
       <c r="A2" s="4">
         <v>1</v>
       </c>
@@ -751,20 +777,21 @@
       <c r="F2" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="G2" s="10" t="s">
+      <c r="G2" s="11" t="s">
         <v>32</v>
       </c>
-      <c r="H2" s="10" t="s">
+      <c r="H2" s="11" t="s">
         <v>37</v>
       </c>
-      <c r="I2" s="10" t="s">
+      <c r="I2" s="11" t="s">
         <v>37</v>
       </c>
-      <c r="J2" s="10" t="s">
-        <v>46</v>
-      </c>
+      <c r="J2" s="11" t="s">
+        <v>45</v>
+      </c>
+      <c r="K2" s="4"/>
     </row>
-    <row r="3" spans="1:10" ht="135" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:11" ht="135" x14ac:dyDescent="0.25">
       <c r="A3" s="4">
         <v>2</v>
       </c>
@@ -783,20 +810,21 @@
       <c r="F3" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="G3" s="10" t="s">
+      <c r="G3" s="11" t="s">
         <v>33</v>
       </c>
-      <c r="H3" s="10" t="s">
+      <c r="H3" s="11" t="s">
         <v>38</v>
       </c>
-      <c r="I3" s="10" t="s">
+      <c r="I3" s="11" t="s">
         <v>44</v>
       </c>
-      <c r="J3" s="1" t="s">
-        <v>47</v>
-      </c>
+      <c r="J3" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="K3" s="4"/>
     </row>
-    <row r="4" spans="1:10" ht="135" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:11" ht="135" x14ac:dyDescent="0.25">
       <c r="A4" s="4">
         <v>3</v>
       </c>
@@ -815,14 +843,19 @@
       <c r="F4" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="G4" s="1" t="s">
+      <c r="G4" s="5" t="s">
         <v>34</v>
       </c>
-      <c r="J4" s="12" t="s">
-        <v>48</v>
+      <c r="H4" s="4"/>
+      <c r="I4" s="4"/>
+      <c r="J4" s="11" t="s">
+        <v>47</v>
+      </c>
+      <c r="K4" s="11" t="s">
+        <v>53</v>
       </c>
     </row>
-    <row r="5" spans="1:10" ht="135" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:11" ht="135" x14ac:dyDescent="0.25">
       <c r="A5" s="4">
         <v>4</v>
       </c>
@@ -841,17 +874,19 @@
       <c r="F5" s="7" t="s">
         <v>30</v>
       </c>
-      <c r="G5" s="11" t="s">
+      <c r="G5" s="12" t="s">
         <v>36</v>
       </c>
-      <c r="I5" s="10" t="s">
+      <c r="H5" s="4"/>
+      <c r="I5" s="11" t="s">
         <v>43</v>
       </c>
-      <c r="J5" s="1" t="s">
-        <v>49</v>
-      </c>
+      <c r="J5" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="K5" s="4"/>
     </row>
-    <row r="6" spans="1:10" ht="75" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:11" ht="75" x14ac:dyDescent="0.25">
       <c r="A6" s="4">
         <v>5</v>
       </c>
@@ -870,20 +905,23 @@
       <c r="F6" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="G6" s="1" t="s">
+      <c r="G6" s="5" t="s">
         <v>35</v>
       </c>
-      <c r="H6" s="12" t="s">
+      <c r="H6" s="11" t="s">
         <v>42</v>
       </c>
-      <c r="I6" s="12" t="s">
+      <c r="I6" s="11" t="s">
         <v>41</v>
       </c>
-      <c r="J6" s="1" t="s">
+      <c r="J6" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="K6" s="11" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="7" spans="1:10" ht="60" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:11" ht="60" x14ac:dyDescent="0.25">
       <c r="A7" s="4">
         <v>6</v>
       </c>
@@ -902,6 +940,11 @@
       <c r="F7" s="5" t="s">
         <v>29</v>
       </c>
+      <c r="G7" s="4"/>
+      <c r="H7" s="4"/>
+      <c r="I7" s="4"/>
+      <c r="J7" s="4"/>
+      <c r="K7" s="4"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
updated the status for 06/04 on behalf of team
</commit_message>
<xml_diff>
--- a/Knowledge Enhancement Plan for the team- draft.xlsx
+++ b/Knowledge Enhancement Plan for the team- draft.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ab70362\Documents\Github\KamnaGupta\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C1AC52AE-13CF-480E-BA83-67387D91FF60}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{22937F04-AB9D-4DC9-9BA9-961845A35958}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="6930" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="75">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="81">
   <si>
     <t>Srinivas</t>
   </si>
@@ -341,12 +341,51 @@
     <t>1. completed writing the stepdefinitions.
 2. worked with srini in connecting the sample web application.</t>
   </si>
+  <si>
+    <t>Latest status as on 6/04</t>
+  </si>
+  <si>
+    <t>1. Implimented running test suite through Jenkins (Through Windows Slave).</t>
+  </si>
+  <si>
+    <t>1. Added code to capture screenshot on a scenario failure.
+2. Tried to add code for extent report generation, but facing some exceptions. Trying to resolve them.</t>
+  </si>
+  <si>
+    <t>on leave</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>UiPath PDF Data Extraction and OCR Data Extraction</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+  </si>
+  <si>
+    <t>1. Was working on CI of Selenium Java project using Maven GIT Jenkins. 
+2. Was looking for Selenium and Jmeter framework. Couldnt find any useful tip.</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -367,6 +406,13 @@
       <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="3">
@@ -434,7 +480,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -455,6 +501,9 @@
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -771,10 +820,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:O7"/>
+  <dimension ref="A1:P7"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="K1" workbookViewId="0">
-      <selection activeCell="O1" sqref="O1"/>
+    <sheetView tabSelected="1" topLeftCell="K6" workbookViewId="0">
+      <selection activeCell="P7" sqref="P7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -797,7 +846,7 @@
     <col min="17" max="16384" width="9.140625" style="7"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" ht="45" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:16" ht="30" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>4</v>
       </c>
@@ -843,8 +892,11 @@
       <c r="O1" s="3" t="s">
         <v>65</v>
       </c>
+      <c r="P1" s="3" t="s">
+        <v>75</v>
+      </c>
     </row>
-    <row r="2" spans="1:15" ht="180" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:16" ht="180" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
         <v>1</v>
       </c>
@@ -890,8 +942,11 @@
       <c r="O2" s="1" t="s">
         <v>69</v>
       </c>
+      <c r="P2" s="7" t="s">
+        <v>76</v>
+      </c>
     </row>
-    <row r="3" spans="1:15" ht="135" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:16" ht="135" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>2</v>
       </c>
@@ -937,8 +992,11 @@
       <c r="O3" s="1" t="s">
         <v>70</v>
       </c>
+      <c r="P3" s="7" t="s">
+        <v>77</v>
+      </c>
     </row>
-    <row r="4" spans="1:15" ht="135" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:16" ht="135" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
         <v>3</v>
       </c>
@@ -980,8 +1038,11 @@
       <c r="O4" s="1" t="s">
         <v>71</v>
       </c>
+      <c r="P4" s="7" t="s">
+        <v>78</v>
+      </c>
     </row>
-    <row r="5" spans="1:15" ht="135" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:16" ht="135" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
         <v>4</v>
       </c>
@@ -1025,8 +1086,11 @@
       <c r="O5" s="1" t="s">
         <v>72</v>
       </c>
+      <c r="P5" s="8" t="s">
+        <v>79</v>
+      </c>
     </row>
-    <row r="6" spans="1:15" ht="90" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:16" ht="90" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
         <v>5</v>
       </c>
@@ -1072,8 +1136,11 @@
       <c r="O6" s="1" t="s">
         <v>67</v>
       </c>
+      <c r="P6" s="7" t="s">
+        <v>80</v>
+      </c>
     </row>
-    <row r="7" spans="1:15" ht="90" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:16" ht="90" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
         <v>6</v>
       </c>

</xml_diff>

<commit_message>
updated on behalf of team for 06/05/2019
</commit_message>
<xml_diff>
--- a/Knowledge Enhancement Plan for the team- draft.xlsx
+++ b/Knowledge Enhancement Plan for the team- draft.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ab70362\Documents\Github\KamnaGupta\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{22937F04-AB9D-4DC9-9BA9-961845A35958}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7EC4D584-1A60-4AB0-AA7E-BBD5731EF026}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="6930" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="81">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="114" uniqueCount="86">
   <si>
     <t>Srinivas</t>
   </si>
@@ -352,9 +352,6 @@
 2. Tried to add code for extent report generation, but facing some exceptions. Trying to resolve them.</t>
   </si>
   <si>
-    <t>on leave</t>
-  </si>
-  <si>
     <r>
       <rPr>
         <sz val="11"/>
@@ -379,6 +376,25 @@
   <si>
     <t>1. Was working on CI of Selenium Java project using Maven GIT Jenkins. 
 2. Was looking for Selenium and Jmeter framework. Couldnt find any useful tip.</t>
+  </si>
+  <si>
+    <t>Latest status as on 6/05</t>
+  </si>
+  <si>
+    <t>1. Extent report generation is still in progress.
+2. Still working on accepting data from the excel sheet.</t>
+  </si>
+  <si>
+    <t>1. Implemented Jenkins with parallel browsing testing.</t>
+  </si>
+  <si>
+    <t>ON LEAVE</t>
+  </si>
+  <si>
+    <t>1. Jmeter PPT preparation.</t>
+  </si>
+  <si>
+    <t>1. Excel and Data Table Automation.</t>
   </si>
 </sst>
 </file>
@@ -480,7 +496,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -503,7 +519,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -820,10 +839,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:P7"/>
+  <dimension ref="A1:Q7"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="K6" workbookViewId="0">
-      <selection activeCell="P7" sqref="P7"/>
+    <sheetView tabSelected="1" topLeftCell="B4" workbookViewId="0">
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -842,11 +861,13 @@
     <col min="12" max="12" width="28" style="7" customWidth="1"/>
     <col min="13" max="13" width="27.140625" style="7" customWidth="1"/>
     <col min="14" max="14" width="33" style="7" customWidth="1"/>
-    <col min="15" max="16" width="27.140625" style="7" customWidth="1"/>
-    <col min="17" max="16384" width="9.140625" style="7"/>
+    <col min="15" max="15" width="27.140625" style="7" customWidth="1"/>
+    <col min="16" max="16" width="23.28515625" style="7" customWidth="1"/>
+    <col min="17" max="17" width="24.28515625" style="7" customWidth="1"/>
+    <col min="18" max="16384" width="9.140625" style="7"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" ht="30" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:17" ht="45" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>4</v>
       </c>
@@ -895,8 +916,11 @@
       <c r="P1" s="3" t="s">
         <v>75</v>
       </c>
+      <c r="Q1" s="3" t="s">
+        <v>80</v>
+      </c>
     </row>
-    <row r="2" spans="1:16" ht="180" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:17" ht="180" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
         <v>1</v>
       </c>
@@ -942,11 +966,14 @@
       <c r="O2" s="1" t="s">
         <v>69</v>
       </c>
-      <c r="P2" s="7" t="s">
+      <c r="P2" s="1" t="s">
         <v>76</v>
       </c>
+      <c r="Q2" s="1" t="s">
+        <v>82</v>
+      </c>
     </row>
-    <row r="3" spans="1:16" ht="135" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:17" ht="210" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>2</v>
       </c>
@@ -992,11 +1019,14 @@
       <c r="O3" s="1" t="s">
         <v>70</v>
       </c>
-      <c r="P3" s="7" t="s">
+      <c r="P3" s="1" t="s">
         <v>77</v>
       </c>
+      <c r="Q3" s="1" t="s">
+        <v>81</v>
+      </c>
     </row>
-    <row r="4" spans="1:16" ht="135" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:17" ht="135" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
         <v>3</v>
       </c>
@@ -1038,11 +1068,14 @@
       <c r="O4" s="1" t="s">
         <v>71</v>
       </c>
-      <c r="P4" s="7" t="s">
-        <v>78</v>
+      <c r="P4" s="8" t="s">
+        <v>83</v>
+      </c>
+      <c r="Q4" s="1" t="s">
+        <v>85</v>
       </c>
     </row>
-    <row r="5" spans="1:16" ht="135" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:17" ht="135" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
         <v>4</v>
       </c>
@@ -1086,11 +1119,14 @@
       <c r="O5" s="1" t="s">
         <v>72</v>
       </c>
-      <c r="P5" s="8" t="s">
-        <v>79</v>
+      <c r="P5" s="9" t="s">
+        <v>78</v>
+      </c>
+      <c r="Q5" s="8" t="s">
+        <v>83</v>
       </c>
     </row>
-    <row r="6" spans="1:16" ht="90" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:17" ht="120" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
         <v>5</v>
       </c>
@@ -1136,11 +1172,14 @@
       <c r="O6" s="1" t="s">
         <v>67</v>
       </c>
-      <c r="P6" s="7" t="s">
-        <v>80</v>
+      <c r="P6" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="Q6" s="1" t="s">
+        <v>84</v>
       </c>
     </row>
-    <row r="7" spans="1:16" ht="90" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:17" ht="90" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
         <v>6</v>
       </c>
@@ -1168,6 +1207,8 @@
       <c r="M7" s="1"/>
       <c r="N7" s="1"/>
       <c r="O7" s="1"/>
+      <c r="P7" s="1"/>
+      <c r="Q7" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Updated status of Nikhil, Srinivas and Ramesh for 06/06/2019
</commit_message>
<xml_diff>
--- a/Knowledge Enhancement Plan for the team- draft.xlsx
+++ b/Knowledge Enhancement Plan for the team- draft.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ab70362\Documents\Github\KamnaGupta\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7EC4D584-1A60-4AB0-AA7E-BBD5731EF026}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C669F143-BA9B-4ACF-AC1D-3FCA07A0E9E6}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="6930" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="114" uniqueCount="86">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="90">
   <si>
     <t>Srinivas</t>
   </si>
@@ -385,9 +385,6 @@
 2. Still working on accepting data from the excel sheet.</t>
   </si>
   <si>
-    <t>1. Implemented Jenkins with parallel browsing testing.</t>
-  </si>
-  <si>
     <t>ON LEAVE</t>
   </si>
   <si>
@@ -395,13 +392,31 @@
   </si>
   <si>
     <t>1. Excel and Data Table Automation.</t>
+  </si>
+  <si>
+    <t>Latest status as on 6/06</t>
+  </si>
+  <si>
+    <t>1. Implemented Jenkins with parallel browser testing.</t>
+  </si>
+  <si>
+    <t>1. IN PROGRESS- Adding the git repository to Jenkins.
+2. Cucumber framework with Data Driven and POM is in progress.</t>
+  </si>
+  <si>
+    <t>1. Implemented extent reports in the project and reports are getting generated as per the result.
+2. Trying to add the screenshots in failure case to the extent reports.
+3. Accepting input from the excel sheet is still in progress.</t>
+  </si>
+  <si>
+    <t>1. Reading Email and Deleting automatically through RPA.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -429,6 +444,12 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Segoe UI"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="3">
@@ -496,7 +517,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -524,6 +545,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -839,10 +863,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:Q7"/>
+  <dimension ref="A1:R7"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B4" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+    <sheetView tabSelected="1" topLeftCell="L5" workbookViewId="0">
+      <selection activeCell="R6" sqref="R6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -864,10 +888,11 @@
     <col min="15" max="15" width="27.140625" style="7" customWidth="1"/>
     <col min="16" max="16" width="23.28515625" style="7" customWidth="1"/>
     <col min="17" max="17" width="24.28515625" style="7" customWidth="1"/>
-    <col min="18" max="16384" width="9.140625" style="7"/>
+    <col min="18" max="18" width="23.140625" style="7" customWidth="1"/>
+    <col min="19" max="16384" width="9.140625" style="7"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" ht="45" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:18" ht="45" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>4</v>
       </c>
@@ -919,8 +944,11 @@
       <c r="Q1" s="3" t="s">
         <v>80</v>
       </c>
+      <c r="R1" s="3" t="s">
+        <v>85</v>
+      </c>
     </row>
-    <row r="2" spans="1:17" ht="180" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:18" ht="180" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
         <v>1</v>
       </c>
@@ -970,10 +998,13 @@
         <v>76</v>
       </c>
       <c r="Q2" s="1" t="s">
-        <v>82</v>
+        <v>86</v>
+      </c>
+      <c r="R2" s="7" t="s">
+        <v>87</v>
       </c>
     </row>
-    <row r="3" spans="1:17" ht="210" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:18" ht="180" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>2</v>
       </c>
@@ -1025,8 +1056,11 @@
       <c r="Q3" s="1" t="s">
         <v>81</v>
       </c>
+      <c r="R3" s="7" t="s">
+        <v>88</v>
+      </c>
     </row>
-    <row r="4" spans="1:17" ht="135" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:18" ht="135" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
         <v>3</v>
       </c>
@@ -1069,13 +1103,16 @@
         <v>71</v>
       </c>
       <c r="P4" s="8" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="Q4" s="1" t="s">
-        <v>85</v>
+        <v>84</v>
+      </c>
+      <c r="R4" s="10" t="s">
+        <v>89</v>
       </c>
     </row>
-    <row r="5" spans="1:17" ht="135" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:18" ht="135" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
         <v>4</v>
       </c>
@@ -1123,10 +1160,13 @@
         <v>78</v>
       </c>
       <c r="Q5" s="8" t="s">
-        <v>83</v>
+        <v>82</v>
+      </c>
+      <c r="R5" s="8" t="s">
+        <v>82</v>
       </c>
     </row>
-    <row r="6" spans="1:17" ht="120" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:18" ht="120" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
         <v>5</v>
       </c>
@@ -1176,10 +1216,10 @@
         <v>79</v>
       </c>
       <c r="Q6" s="1" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
-    <row r="7" spans="1:17" ht="90" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:18" ht="90" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
         <v>6</v>
       </c>

</xml_diff>

<commit_message>
updated on behalf of team for 06/07/2019
</commit_message>
<xml_diff>
--- a/Knowledge Enhancement Plan for the team- draft.xlsx
+++ b/Knowledge Enhancement Plan for the team- draft.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\GITHUB\KamnaGupta\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ab70362\Documents\Github\KamnaGupta\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0DB38C5E-668D-42E2-AFAC-6ED473514515}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C51F46AC-AE8A-4D85-9153-3D0417D17410}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="6930" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="91">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="110" uniqueCount="96">
   <si>
     <t>Srinivas</t>
   </si>
@@ -414,6 +414,23 @@
   <si>
     <t>Working on extent report and CI part of Selenium Project.
 Tried to do more for Jmeter, couldn't find much help.</t>
+  </si>
+  <si>
+    <t>Latest status as on 6/07</t>
+  </si>
+  <si>
+    <t>1. Installed Jenkins.
+2. Adding the screenshot to the extent report is still in progress.</t>
+  </si>
+  <si>
+    <t>1.  Data scraping of e-commerce webpages</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1. Excel Automation and activities 
+ </t>
+  </si>
+  <si>
+    <t>1. Prepared step definitions for the sample website in cucumber framework.</t>
   </si>
 </sst>
 </file>
@@ -550,8 +567,8 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -867,10 +884,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:R7"/>
+  <dimension ref="A1:S7"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="L6" workbookViewId="0">
-      <selection activeCell="R6" sqref="R6"/>
+    <sheetView tabSelected="1" topLeftCell="M1" workbookViewId="0">
+      <selection activeCell="S2" sqref="S2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -892,11 +909,11 @@
     <col min="15" max="15" width="27.140625" style="7" customWidth="1"/>
     <col min="16" max="16" width="23.28515625" style="7" customWidth="1"/>
     <col min="17" max="17" width="24.28515625" style="7" customWidth="1"/>
-    <col min="18" max="18" width="23.140625" style="7" customWidth="1"/>
-    <col min="19" max="16384" width="9.140625" style="7"/>
+    <col min="18" max="19" width="23.140625" style="7" customWidth="1"/>
+    <col min="20" max="16384" width="9.140625" style="7"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" ht="45" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:19" ht="45" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>4</v>
       </c>
@@ -951,8 +968,11 @@
       <c r="R1" s="3" t="s">
         <v>85</v>
       </c>
+      <c r="S1" s="3" t="s">
+        <v>91</v>
+      </c>
     </row>
-    <row r="2" spans="1:18" ht="180" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:19" ht="180" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
         <v>1</v>
       </c>
@@ -1004,11 +1024,14 @@
       <c r="Q2" s="1" t="s">
         <v>86</v>
       </c>
-      <c r="R2" s="7" t="s">
+      <c r="R2" s="1" t="s">
         <v>87</v>
       </c>
+      <c r="S2" s="1" t="s">
+        <v>95</v>
+      </c>
     </row>
-    <row r="3" spans="1:18" ht="180" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:19" ht="180" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>2</v>
       </c>
@@ -1060,11 +1083,14 @@
       <c r="Q3" s="1" t="s">
         <v>81</v>
       </c>
-      <c r="R3" s="7" t="s">
+      <c r="R3" s="1" t="s">
         <v>88</v>
       </c>
+      <c r="S3" s="1" t="s">
+        <v>92</v>
+      </c>
     </row>
-    <row r="4" spans="1:18" ht="135" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:19" ht="135" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
         <v>3</v>
       </c>
@@ -1115,8 +1141,11 @@
       <c r="R4" s="10" t="s">
         <v>89</v>
       </c>
+      <c r="S4" s="1" t="s">
+        <v>93</v>
+      </c>
     </row>
-    <row r="5" spans="1:18" ht="135" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:19" ht="135" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
         <v>4</v>
       </c>
@@ -1169,8 +1198,11 @@
       <c r="R5" s="8" t="s">
         <v>82</v>
       </c>
+      <c r="S5" s="1" t="s">
+        <v>94</v>
+      </c>
     </row>
-    <row r="6" spans="1:18" ht="120" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:19" ht="120" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
         <v>5</v>
       </c>
@@ -1222,11 +1254,12 @@
       <c r="Q6" s="1" t="s">
         <v>83</v>
       </c>
-      <c r="R6" s="7" t="s">
+      <c r="R6" s="1" t="s">
         <v>90</v>
       </c>
+      <c r="S6" s="1"/>
     </row>
-    <row r="7" spans="1:18" ht="90" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:19" ht="90" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
         <v>6</v>
       </c>
@@ -1256,6 +1289,8 @@
       <c r="O7" s="1"/>
       <c r="P7" s="1"/>
       <c r="Q7" s="1"/>
+      <c r="R7" s="1"/>
+      <c r="S7" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>